<commit_message>
rettelse til aktør kontekst diagram
</commit_message>
<xml_diff>
--- a/tidsplan.xlsx
+++ b/tidsplan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lív Hansen\Google Drive\Skúli\Semester 4\EE4PRJ Projekt 4\Semesterprojekt4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Dokumenter\skole\F18\projekt\Semesterprojekt4\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="FD593637D7F48F58C4F9985D2B64B3A01C30876C" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{D9B847D9-9169-46D1-9791-82BE84B6D480}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -113,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -256,13 +257,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,9 +293,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kontor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -332,7 +333,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kontor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -438,7 +439,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kontor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -587,19 +588,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,7 +653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -673,7 +674,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -694,7 +695,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -715,7 +716,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -736,7 +737,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -757,7 +758,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -778,7 +779,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -797,7 +798,7 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -818,7 +819,7 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -839,7 +840,7 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>22</v>
       </c>
@@ -860,7 +861,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>23</v>
       </c>
@@ -881,7 +882,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>24</v>
       </c>
@@ -902,7 +903,7 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>25</v>
       </c>
@@ -912,7 +913,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="17" t="s">
         <v>27</v>
       </c>
       <c r="I14" s="5"/>
@@ -925,7 +926,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -933,7 +934,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="15"/>
+      <c r="H15" s="17"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -944,7 +945,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -954,7 +955,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="15"/>
+      <c r="H16" s="17"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -965,7 +966,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -975,7 +976,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="15"/>
+      <c r="H17" s="17"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -986,7 +987,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -996,7 +997,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="15"/>
+      <c r="H18" s="17"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -1007,7 +1008,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1015,7 +1016,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="15"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -1026,7 +1027,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1036,7 +1037,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="15"/>
+      <c r="H20" s="17"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -1047,7 +1048,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1057,7 +1058,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="15"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="5"/>
@@ -1068,7 +1069,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -1078,7 +1079,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="15"/>
+      <c r="H22" s="17"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="5"/>
@@ -1089,7 +1090,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1097,7 +1098,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="15"/>
+      <c r="H23" s="17"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -1108,7 +1109,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
@@ -1131,7 +1132,7 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -1152,7 +1153,7 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1174,7 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
@@ -1194,7 +1195,7 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1213,7 +1214,7 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
@@ -1234,7 +1235,7 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
@@ -1255,7 +1256,7 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
@@ -1276,7 +1277,7 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1298,7 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1316,7 +1317,7 @@
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -1337,26 +1338,26 @@
       <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>